<commit_message>
update interview score docs
</commit_message>
<xml_diff>
--- a/scores/면접평가서.xlsx
+++ b/scores/면접평가서.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekank\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\side\frontend-interview\scores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C3AE25-619E-4735-B708-C49A28675330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED92085F-805F-4573-9AAD-B21D355D84B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3780" yWindow="585" windowWidth="21600" windowHeight="14625" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>종합 의견</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -89,22 +89,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>변수 관련 코딩 문제</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>this 관련 코딩 문제</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>JS 동작 원리 관련 코딩 문제</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>JS 동작 원리 관련 코딩 문제 2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>React 사용 이유</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -169,15 +153,19 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>React 기본 코딩 질문</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TS 관련 코딩 질문</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>확장성 관련 코딩 질문</t>
+    <t>라이브 코딩 문제 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>라이브 코딩 문제 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>라이브 코딩 문제 3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>라이브 코딩 문제 4</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -514,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -529,126 +517,123 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -954,8 +939,8 @@
   </sheetPr>
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -971,13 +956,13 @@
       <c r="A2" s="1"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="46"/>
+      <c r="D2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="29"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -987,295 +972,295 @@
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="78" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
+      <c r="B3" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="1:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="42" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="43"/>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="24" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="17"/>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="45"/>
+      <c r="C6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="17"/>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="45"/>
+      <c r="C7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:13" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="31"/>
+      <c r="C8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="45"/>
+      <c r="C10" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-    </row>
-    <row r="8" spans="1:13" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="21"/>
-      <c r="C8" s="22" t="s">
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+    </row>
+    <row r="11" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="45"/>
+      <c r="C11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="45"/>
+      <c r="C12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:13" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="31"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-    </row>
-    <row r="9" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="45"/>
+      <c r="C15" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="45"/>
+      <c r="C16" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="45"/>
+      <c r="C17" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="45"/>
+      <c r="C18" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+    </row>
+    <row r="19" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="45"/>
+      <c r="C19" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="45"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="2:6" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="31"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="45"/>
+      <c r="C23" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="45"/>
+      <c r="C24" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-    </row>
-    <row r="10" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="17"/>
-      <c r="C10" s="41" t="s">
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="45"/>
+      <c r="C25" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+    </row>
+    <row r="26" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="45"/>
+      <c r="C26" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-    </row>
-    <row r="11" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="17"/>
-      <c r="C11" s="20" t="s">
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="45"/>
+      <c r="C27" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-    </row>
-    <row r="12" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="17"/>
-      <c r="C12" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" spans="1:13" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-    </row>
-    <row r="14" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="25" t="s">
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" spans="2:6" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="31"/>
+      <c r="C28" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-    </row>
-    <row r="15" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="17"/>
-      <c r="C15" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-    </row>
-    <row r="16" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="17"/>
-      <c r="C16" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-    </row>
-    <row r="17" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="17"/>
-      <c r="C17" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-    </row>
-    <row r="18" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="17"/>
-      <c r="C18" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-    </row>
-    <row r="19" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="17"/>
-      <c r="C19" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-    </row>
-    <row r="20" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="17"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-    </row>
-    <row r="21" spans="2:6" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="21"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-    </row>
-    <row r="22" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-    </row>
-    <row r="23" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="17"/>
-      <c r="C23" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="17"/>
-      <c r="C24" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-    </row>
-    <row r="25" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="17"/>
-      <c r="C25" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-    </row>
-    <row r="26" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="17"/>
-      <c r="C26" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-    </row>
-    <row r="27" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="17"/>
-      <c r="C27" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-    </row>
-    <row r="28" spans="2:6" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="21"/>
-      <c r="C28" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
+      <c r="B29" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="33"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
     </row>
     <row r="30" spans="2:6" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="21"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
     </row>
     <row r="31" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
     </row>
     <row r="32" spans="2:6" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="21"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
     </row>
     <row r="33" spans="1:7" ht="34.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="8"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="6"/>
     </row>
     <row r="34" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="8"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="6"/>
     </row>
     <row r="36" spans="1:7" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36"/>
@@ -1285,6 +1270,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="B22:B28"/>
     <mergeCell ref="B33:F34"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="B29:B30"/>
@@ -1301,8 +1288,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="B9:B13"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="B22:B28"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>